<commit_message>
Update the summary of findings
</commit_message>
<xml_diff>
--- a/Findings Summary.xlsx
+++ b/Findings Summary.xlsx
@@ -11,6 +11,22 @@
   <definedNames/>
   <calcPr/>
 </workbook>
+</file>
+
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="A1">
+      <text>
+        <t xml:space="preserve">fantastic work!
+	-Sylvia Kreibig</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2002,9 +2018,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4876800" cy="4200525"/>
     <xdr:pic>
@@ -42412,7 +42428,8 @@
     <mergeCell ref="A80:D80"/>
     <mergeCell ref="E80:H80"/>
   </mergeCells>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>